<commit_message>
replace color tap NCKH 2007
</commit_message>
<xml_diff>
--- a/NCKH_2017_CNTT.xlsx
+++ b/NCKH_2017_CNTT.xlsx
@@ -453,7 +453,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -547,7 +547,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,6 +828,8 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -855,8 +857,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1247,7 +1247,7 @@
   <dimension ref="A1:AN4654"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,20 +1264,20 @@
     <col min="11" max="11" width="13.44140625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1309,19 +1309,19 @@
       <c r="AN1" s="2"/>
     </row>
     <row r="2" spans="1:40" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1395,19 +1395,19 @@
       <c r="AN3" s="2"/>
     </row>
     <row r="4" spans="1:40" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1455,10 +1455,10 @@
       <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="6" t="s">
         <v>58</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>90</v>
       </c>
       <c r="J12" s="39">
-        <f t="shared" ref="J9:J12" si="0">H12-I12</f>
+        <f t="shared" ref="J12" si="0">H12-I12</f>
         <v>-78</v>
       </c>
       <c r="K12" s="19"/>
@@ -3305,14 +3305,14 @@
       <c r="C38" s="10"/>
       <c r="D38" s="53"/>
       <c r="E38" s="54"/>
-      <c r="F38" s="72" t="s">
+      <c r="F38" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="G38" s="72"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3349,14 +3349,14 @@
       <c r="C39" s="10"/>
       <c r="D39" s="55"/>
       <c r="E39" s="53"/>
-      <c r="F39" s="64" t="s">
+      <c r="F39" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="64"/>
-      <c r="J39" s="64"/>
-      <c r="K39" s="64"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="66"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3561,12 +3561,12 @@
       <c r="C44" s="10"/>
       <c r="D44" s="1"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="65"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="65"/>
-      <c r="K44" s="65"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -22985,7 +22985,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D1" s="73"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="50"/>
@@ -22994,7 +22994,7 @@
     <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
-      <c r="D3" s="74"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="50"/>
@@ -23080,43 +23080,43 @@
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
     </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
     </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
     </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
     </row>
-    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
     </row>
-    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
     </row>
-    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="50"/>
       <c r="C31" s="50"/>
     </row>
-    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="50"/>
       <c r="C32" s="50"/>
     </row>
-    <row r="33" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="50"/>
       <c r="C33" s="50"/>
     </row>
-    <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="50"/>
       <c r="C34" s="50"/>
     </row>

</xml_diff>